<commit_message>
Updated VarCosts to all combinations
</commit_message>
<xml_diff>
--- a/varCosts.xlsx
+++ b/varCosts.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:F17"/>
+  <dimension ref="A1:F101"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -473,20 +473,20 @@
       </c>
       <c r="B2" t="inlineStr">
         <is>
-          <t>P1</t>
+          <t>C1</t>
         </is>
       </c>
       <c r="C2" t="n">
-        <v>180.0504633685024</v>
+        <v>0</v>
       </c>
       <c r="D2" t="n">
-        <v>64.68348778950079</v>
+        <v>0</v>
       </c>
       <c r="E2" t="n">
-        <v>90.0252316842512</v>
+        <v>0</v>
       </c>
       <c r="F2" t="n">
-        <v>154.708719473752</v>
+        <v>0</v>
       </c>
     </row>
     <row r="3">
@@ -497,356 +497,2372 @@
       </c>
       <c r="B3" t="inlineStr">
         <is>
-          <t>P2</t>
+          <t>C2</t>
         </is>
       </c>
       <c r="C3" t="n">
-        <v>50.61327616095006</v>
+        <v>39.10398995515984</v>
       </c>
       <c r="D3" t="n">
-        <v>21.53775872031669</v>
+        <v>17.70132998505328</v>
       </c>
       <c r="E3" t="n">
-        <v>25.30663808047503</v>
+        <v>19.55199497757992</v>
       </c>
       <c r="F3" t="n">
-        <v>46.84439680079171</v>
+        <v>37.2533249626332</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" t="inlineStr">
         <is>
-          <t>C2</t>
+          <t>C1</t>
         </is>
       </c>
       <c r="B4" t="inlineStr">
         <is>
-          <t>P1</t>
+          <t>C3</t>
         </is>
       </c>
       <c r="C4" t="n">
-        <v>142.7763334018379</v>
+        <v>121.6848783668781</v>
       </c>
       <c r="D4" t="n">
-        <v>52.25877780061261</v>
+        <v>45.22829278895937</v>
       </c>
       <c r="E4" t="n">
-        <v>71.38816670091893</v>
+        <v>60.84243918343906</v>
       </c>
       <c r="F4" t="n">
-        <v>123.6469445015316</v>
+        <v>106.0707319723984</v>
       </c>
     </row>
     <row r="5">
       <c r="A5" t="inlineStr">
         <is>
-          <t>C2</t>
+          <t>C1</t>
         </is>
       </c>
       <c r="B5" t="inlineStr">
         <is>
-          <t>P2</t>
+          <t>P1</t>
         </is>
       </c>
       <c r="C5" t="n">
-        <v>67.95730255244631</v>
+        <v>180.0504633685024</v>
       </c>
       <c r="D5" t="n">
-        <v>27.31910085081544</v>
+        <v>64.68348778950079</v>
       </c>
       <c r="E5" t="n">
-        <v>33.97865127622315</v>
+        <v>90.0252316842512</v>
       </c>
       <c r="F5" t="n">
-        <v>61.29775212703859</v>
+        <v>154.708719473752</v>
       </c>
     </row>
     <row r="6">
       <c r="A6" t="inlineStr">
         <is>
-          <t>C3</t>
+          <t>C1</t>
         </is>
       </c>
       <c r="B6" t="inlineStr">
         <is>
-          <t>P1</t>
+          <t>P2</t>
         </is>
       </c>
       <c r="C6" t="n">
-        <v>62.92204263053249</v>
+        <v>50.61327616095006</v>
       </c>
       <c r="D6" t="n">
-        <v>25.64068087684416</v>
+        <v>21.53775872031669</v>
       </c>
       <c r="E6" t="n">
-        <v>31.46102131526624</v>
+        <v>25.30663808047503</v>
       </c>
       <c r="F6" t="n">
-        <v>57.10170219211041</v>
+        <v>46.84439680079171</v>
       </c>
     </row>
     <row r="7">
       <c r="A7" t="inlineStr">
         <is>
-          <t>C3</t>
+          <t>C1</t>
         </is>
       </c>
       <c r="B7" t="inlineStr">
         <is>
-          <t>P2</t>
+          <t>S1</t>
         </is>
       </c>
       <c r="C7" t="n">
-        <v>154.8036398937564</v>
+        <v>1159.566772494025</v>
       </c>
       <c r="D7" t="n">
-        <v>56.26787996458545</v>
+        <v>391.1889241646749</v>
       </c>
       <c r="E7" t="n">
-        <v>77.40181994687818</v>
+        <v>579.7833862470123</v>
       </c>
       <c r="F7" t="n">
-        <v>133.6696999114636</v>
+        <v>970.9723104116872</v>
       </c>
     </row>
     <row r="8">
       <c r="A8" t="inlineStr">
         <is>
-          <t>P1</t>
+          <t>C1</t>
         </is>
       </c>
       <c r="B8" t="inlineStr">
         <is>
-          <t>S1</t>
+          <t>S2</t>
         </is>
       </c>
       <c r="C8" t="n">
-        <v>1296.317108197894</v>
+        <v>206.7285173493552</v>
       </c>
       <c r="D8" t="n">
-        <v>436.772369399298</v>
+        <v>73.57617244978508</v>
       </c>
       <c r="E8" t="n">
-        <v>648.158554098947</v>
+        <v>103.3642586746776</v>
       </c>
       <c r="F8" t="n">
-        <v>1084.930923498245</v>
+        <v>176.9404311244627</v>
       </c>
     </row>
     <row r="9">
       <c r="A9" t="inlineStr">
         <is>
-          <t>P1</t>
+          <t>C1</t>
         </is>
       </c>
       <c r="B9" t="inlineStr">
         <is>
-          <t>S2</t>
+          <t>S3</t>
         </is>
       </c>
       <c r="C9" t="n">
-        <v>208.7845964459393</v>
+        <v>65.89157990019301</v>
       </c>
       <c r="D9" t="n">
-        <v>74.26153214864644</v>
+        <v>26.63052663339767</v>
       </c>
       <c r="E9" t="n">
-        <v>104.3922982229697</v>
+        <v>32.9457899500965</v>
       </c>
       <c r="F9" t="n">
-        <v>178.6538303716161</v>
+        <v>59.57631658349418</v>
       </c>
     </row>
     <row r="10">
       <c r="A10" t="inlineStr">
         <is>
-          <t>P1</t>
+          <t>C1</t>
         </is>
       </c>
       <c r="B10" t="inlineStr">
         <is>
-          <t>S3</t>
+          <t>S4</t>
         </is>
       </c>
       <c r="C10" t="n">
-        <v>192.7915133234025</v>
+        <v>191.3610883898892</v>
       </c>
       <c r="D10" t="n">
-        <v>68.93050444113416</v>
+        <v>68.45369612996306</v>
       </c>
       <c r="E10" t="n">
-        <v>96.39575666170124</v>
+        <v>95.68054419494459</v>
       </c>
       <c r="F10" t="n">
-        <v>165.3262611028354</v>
+        <v>164.1342403249076</v>
       </c>
     </row>
     <row r="11">
       <c r="A11" t="inlineStr">
         <is>
-          <t>P1</t>
+          <t>C1</t>
         </is>
       </c>
       <c r="B11" t="inlineStr">
         <is>
-          <t>S4</t>
+          <t>S5</t>
         </is>
       </c>
       <c r="C11" t="n">
-        <v>79.35219477451162</v>
+        <v>71.95941646118726</v>
       </c>
       <c r="D11" t="n">
-        <v>31.11739825817054</v>
+        <v>28.65313882039575</v>
       </c>
       <c r="E11" t="n">
-        <v>39.67609738725581</v>
+        <v>35.97970823059363</v>
       </c>
       <c r="F11" t="n">
-        <v>70.79349564542635</v>
+        <v>64.63284705098938</v>
       </c>
     </row>
     <row r="12">
       <c r="A12" t="inlineStr">
         <is>
-          <t>P1</t>
+          <t>C2</t>
         </is>
       </c>
       <c r="B12" t="inlineStr">
         <is>
-          <t>S5</t>
+          <t>C1</t>
         </is>
       </c>
       <c r="C12" t="n">
-        <v>211.7734838345068</v>
+        <v>39.10398995515984</v>
       </c>
       <c r="D12" t="n">
-        <v>75.2578279448356</v>
+        <v>17.70132998505328</v>
       </c>
       <c r="E12" t="n">
-        <v>105.8867419172534</v>
+        <v>19.55199497757992</v>
       </c>
       <c r="F12" t="n">
-        <v>181.144569862089</v>
+        <v>37.2533249626332</v>
       </c>
     </row>
     <row r="13">
       <c r="A13" t="inlineStr">
         <is>
-          <t>P2</t>
+          <t>C2</t>
         </is>
       </c>
       <c r="B13" t="inlineStr">
         <is>
-          <t>S1</t>
+          <t>C2</t>
         </is>
       </c>
       <c r="C13" t="n">
-        <v>1113.287259822019</v>
+        <v>0</v>
       </c>
       <c r="D13" t="n">
-        <v>375.7624199406728</v>
+        <v>0</v>
       </c>
       <c r="E13" t="n">
-        <v>556.6436299110093</v>
+        <v>0</v>
       </c>
       <c r="F13" t="n">
-        <v>932.4060498516822</v>
+        <v>0</v>
       </c>
     </row>
     <row r="14">
       <c r="A14" t="inlineStr">
         <is>
-          <t>P2</t>
+          <t>C2</t>
         </is>
       </c>
       <c r="B14" t="inlineStr">
         <is>
-          <t>S2</t>
+          <t>C3</t>
         </is>
       </c>
       <c r="C14" t="n">
-        <v>257.3213824259944</v>
+        <v>87.70109921810007</v>
       </c>
       <c r="D14" t="n">
-        <v>90.4404608086648</v>
+        <v>33.90036640603336</v>
       </c>
       <c r="E14" t="n">
-        <v>128.6606912129972</v>
+        <v>43.85054960905003</v>
       </c>
       <c r="F14" t="n">
-        <v>219.101152021662</v>
+        <v>77.75091601508339</v>
       </c>
     </row>
     <row r="15">
       <c r="A15" t="inlineStr">
         <is>
-          <t>P2</t>
+          <t>C2</t>
         </is>
       </c>
       <c r="B15" t="inlineStr">
         <is>
-          <t>S3</t>
+          <t>P1</t>
         </is>
       </c>
       <c r="C15" t="n">
-        <v>27.03932508674182</v>
+        <v>142.7763334018379</v>
       </c>
       <c r="D15" t="n">
-        <v>13.67977502891394</v>
+        <v>52.25877780061261</v>
       </c>
       <c r="E15" t="n">
-        <v>13.51966254337091</v>
+        <v>71.38816670091893</v>
       </c>
       <c r="F15" t="n">
-        <v>27.19943757228485</v>
+        <v>123.6469445015316</v>
       </c>
     </row>
     <row r="16">
       <c r="A16" t="inlineStr">
         <is>
+          <t>C2</t>
+        </is>
+      </c>
+      <c r="B16" t="inlineStr">
+        <is>
           <t>P2</t>
         </is>
       </c>
-      <c r="B16" t="inlineStr">
-        <is>
-          <t>S4</t>
-        </is>
-      </c>
       <c r="C16" t="n">
-        <v>196.9396303888934</v>
+        <v>67.95730255244631</v>
       </c>
       <c r="D16" t="n">
-        <v>70.31321012963113</v>
+        <v>27.31910085081544</v>
       </c>
       <c r="E16" t="n">
-        <v>98.4698151944467</v>
+        <v>33.97865127622315</v>
       </c>
       <c r="F16" t="n">
-        <v>168.7830253240778</v>
+        <v>61.29775212703859</v>
       </c>
     </row>
     <row r="17">
       <c r="A17" t="inlineStr">
         <is>
+          <t>C2</t>
+        </is>
+      </c>
+      <c r="B17" t="inlineStr">
+        <is>
+          <t>S1</t>
+        </is>
+      </c>
+      <c r="C17" t="n">
+        <v>1180.196966276215</v>
+      </c>
+      <c r="D17" t="n">
+        <v>398.0656554254051</v>
+      </c>
+      <c r="E17" t="n">
+        <v>590.0984831381077</v>
+      </c>
+      <c r="F17" t="n">
+        <v>988.1641385635128</v>
+      </c>
+    </row>
+    <row r="18">
+      <c r="A18" t="inlineStr">
+        <is>
+          <t>C2</t>
+        </is>
+      </c>
+      <c r="B18" t="inlineStr">
+        <is>
+          <t>S2</t>
+        </is>
+      </c>
+      <c r="C18" t="n">
+        <v>203.9719900298204</v>
+      </c>
+      <c r="D18" t="n">
+        <v>72.65733000994013</v>
+      </c>
+      <c r="E18" t="n">
+        <v>101.9859950149102</v>
+      </c>
+      <c r="F18" t="n">
+        <v>174.6433250248503</v>
+      </c>
+    </row>
+    <row r="19">
+      <c r="A19" t="inlineStr">
+        <is>
+          <t>C2</t>
+        </is>
+      </c>
+      <c r="B19" t="inlineStr">
+        <is>
+          <t>S3</t>
+        </is>
+      </c>
+      <c r="C19" t="n">
+        <v>67.60376858924941</v>
+      </c>
+      <c r="D19" t="n">
+        <v>27.20125619641647</v>
+      </c>
+      <c r="E19" t="n">
+        <v>33.80188429462471</v>
+      </c>
+      <c r="F19" t="n">
+        <v>61.00314049104118</v>
+      </c>
+    </row>
+    <row r="20">
+      <c r="A20" t="inlineStr">
+        <is>
+          <t>C2</t>
+        </is>
+      </c>
+      <c r="B20" t="inlineStr">
+        <is>
+          <t>S4</t>
+        </is>
+      </c>
+      <c r="C20" t="n">
+        <v>152.8377121278224</v>
+      </c>
+      <c r="D20" t="n">
+        <v>55.61257070927415</v>
+      </c>
+      <c r="E20" t="n">
+        <v>76.41885606391122</v>
+      </c>
+      <c r="F20" t="n">
+        <v>132.0314267731854</v>
+      </c>
+    </row>
+    <row r="21">
+      <c r="A21" t="inlineStr">
+        <is>
+          <t>C2</t>
+        </is>
+      </c>
+      <c r="B21" t="inlineStr">
+        <is>
+          <t>S5</t>
+        </is>
+      </c>
+      <c r="C21" t="n">
+        <v>82.28463421703982</v>
+      </c>
+      <c r="D21" t="n">
+        <v>32.0948780723466</v>
+      </c>
+      <c r="E21" t="n">
+        <v>41.14231710851991</v>
+      </c>
+      <c r="F21" t="n">
+        <v>73.23719518086651</v>
+      </c>
+    </row>
+    <row r="22">
+      <c r="A22" t="inlineStr">
+        <is>
+          <t>C3</t>
+        </is>
+      </c>
+      <c r="B22" t="inlineStr">
+        <is>
+          <t>C1</t>
+        </is>
+      </c>
+      <c r="C22" t="n">
+        <v>121.6848783668781</v>
+      </c>
+      <c r="D22" t="n">
+        <v>45.22829278895937</v>
+      </c>
+      <c r="E22" t="n">
+        <v>60.84243918343906</v>
+      </c>
+      <c r="F22" t="n">
+        <v>106.0707319723984</v>
+      </c>
+    </row>
+    <row r="23">
+      <c r="A23" t="inlineStr">
+        <is>
+          <t>C3</t>
+        </is>
+      </c>
+      <c r="B23" t="inlineStr">
+        <is>
+          <t>C2</t>
+        </is>
+      </c>
+      <c r="C23" t="n">
+        <v>87.70109921810007</v>
+      </c>
+      <c r="D23" t="n">
+        <v>33.90036640603336</v>
+      </c>
+      <c r="E23" t="n">
+        <v>43.85054960905003</v>
+      </c>
+      <c r="F23" t="n">
+        <v>77.75091601508339</v>
+      </c>
+    </row>
+    <row r="24">
+      <c r="A24" t="inlineStr">
+        <is>
+          <t>C3</t>
+        </is>
+      </c>
+      <c r="B24" t="inlineStr">
+        <is>
+          <t>C3</t>
+        </is>
+      </c>
+      <c r="C24" t="n">
+        <v>0</v>
+      </c>
+      <c r="D24" t="n">
+        <v>0</v>
+      </c>
+      <c r="E24" t="n">
+        <v>0</v>
+      </c>
+      <c r="F24" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="25">
+      <c r="A25" t="inlineStr">
+        <is>
+          <t>C3</t>
+        </is>
+      </c>
+      <c r="B25" t="inlineStr">
+        <is>
+          <t>P1</t>
+        </is>
+      </c>
+      <c r="C25" t="n">
+        <v>62.92204263053249</v>
+      </c>
+      <c r="D25" t="n">
+        <v>25.64068087684416</v>
+      </c>
+      <c r="E25" t="n">
+        <v>31.46102131526624</v>
+      </c>
+      <c r="F25" t="n">
+        <v>57.10170219211041</v>
+      </c>
+    </row>
+    <row r="26">
+      <c r="A26" t="inlineStr">
+        <is>
+          <t>C3</t>
+        </is>
+      </c>
+      <c r="B26" t="inlineStr">
+        <is>
           <t>P2</t>
         </is>
       </c>
-      <c r="B17" t="inlineStr">
+      <c r="C26" t="n">
+        <v>154.8036398937564</v>
+      </c>
+      <c r="D26" t="n">
+        <v>56.26787996458545</v>
+      </c>
+      <c r="E26" t="n">
+        <v>77.40181994687818</v>
+      </c>
+      <c r="F26" t="n">
+        <v>133.6696999114636</v>
+      </c>
+    </row>
+    <row r="27">
+      <c r="A27" t="inlineStr">
+        <is>
+          <t>C3</t>
+        </is>
+      </c>
+      <c r="B27" t="inlineStr">
+        <is>
+          <t>S1</t>
+        </is>
+      </c>
+      <c r="C27" t="n">
+        <v>1261.990415402678</v>
+      </c>
+      <c r="D27" t="n">
+        <v>425.3301384675593</v>
+      </c>
+      <c r="E27" t="n">
+        <v>630.995207701339</v>
+      </c>
+      <c r="F27" t="n">
+        <v>1056.325346168898</v>
+      </c>
+    </row>
+    <row r="28">
+      <c r="A28" t="inlineStr">
+        <is>
+          <t>C3</t>
+        </is>
+      </c>
+      <c r="B28" t="inlineStr">
+        <is>
+          <t>S2</t>
+        </is>
+      </c>
+      <c r="C28" t="n">
+        <v>171.0808992653463</v>
+      </c>
+      <c r="D28" t="n">
+        <v>61.69363308844878</v>
+      </c>
+      <c r="E28" t="n">
+        <v>85.54044963267316</v>
+      </c>
+      <c r="F28" t="n">
+        <v>147.2340827211219</v>
+      </c>
+    </row>
+    <row r="29">
+      <c r="A29" t="inlineStr">
+        <is>
+          <t>C3</t>
+        </is>
+      </c>
+      <c r="B29" t="inlineStr">
+        <is>
+          <t>S3</t>
+        </is>
+      </c>
+      <c r="C29" t="n">
+        <v>148.1909253635272</v>
+      </c>
+      <c r="D29" t="n">
+        <v>54.06364178784239</v>
+      </c>
+      <c r="E29" t="n">
+        <v>74.09546268176359</v>
+      </c>
+      <c r="F29" t="n">
+        <v>128.159104469606</v>
+      </c>
+    </row>
+    <row r="30">
+      <c r="A30" t="inlineStr">
+        <is>
+          <t>C3</t>
+        </is>
+      </c>
+      <c r="B30" t="inlineStr">
+        <is>
+          <t>S4</t>
+        </is>
+      </c>
+      <c r="C30" t="n">
+        <v>112.2871622400843</v>
+      </c>
+      <c r="D30" t="n">
+        <v>42.09572074669477</v>
+      </c>
+      <c r="E30" t="n">
+        <v>56.14358112004216</v>
+      </c>
+      <c r="F30" t="n">
+        <v>98.23930186673694</v>
+      </c>
+    </row>
+    <row r="31">
+      <c r="A31" t="inlineStr">
+        <is>
+          <t>C3</t>
+        </is>
+      </c>
+      <c r="B31" t="inlineStr">
         <is>
           <t>S5</t>
         </is>
       </c>
-      <c r="C17" t="n">
+      <c r="C31" t="n">
+        <v>165.7915884437255</v>
+      </c>
+      <c r="D31" t="n">
+        <v>59.93052948124182</v>
+      </c>
+      <c r="E31" t="n">
+        <v>82.89579422186274</v>
+      </c>
+      <c r="F31" t="n">
+        <v>142.8263237031045</v>
+      </c>
+    </row>
+    <row r="32">
+      <c r="A32" t="inlineStr">
+        <is>
+          <t>P1</t>
+        </is>
+      </c>
+      <c r="B32" t="inlineStr">
+        <is>
+          <t>C1</t>
+        </is>
+      </c>
+      <c r="C32" t="n">
+        <v>180.0504633685024</v>
+      </c>
+      <c r="D32" t="n">
+        <v>64.68348778950079</v>
+      </c>
+      <c r="E32" t="n">
+        <v>90.0252316842512</v>
+      </c>
+      <c r="F32" t="n">
+        <v>154.708719473752</v>
+      </c>
+    </row>
+    <row r="33">
+      <c r="A33" t="inlineStr">
+        <is>
+          <t>P1</t>
+        </is>
+      </c>
+      <c r="B33" t="inlineStr">
+        <is>
+          <t>C2</t>
+        </is>
+      </c>
+      <c r="C33" t="n">
+        <v>142.7763334018379</v>
+      </c>
+      <c r="D33" t="n">
+        <v>52.25877780061261</v>
+      </c>
+      <c r="E33" t="n">
+        <v>71.38816670091893</v>
+      </c>
+      <c r="F33" t="n">
+        <v>123.6469445015316</v>
+      </c>
+    </row>
+    <row r="34">
+      <c r="A34" t="inlineStr">
+        <is>
+          <t>P1</t>
+        </is>
+      </c>
+      <c r="B34" t="inlineStr">
+        <is>
+          <t>C3</t>
+        </is>
+      </c>
+      <c r="C34" t="n">
+        <v>62.92204263053249</v>
+      </c>
+      <c r="D34" t="n">
+        <v>25.64068087684416</v>
+      </c>
+      <c r="E34" t="n">
+        <v>31.46102131526624</v>
+      </c>
+      <c r="F34" t="n">
+        <v>57.10170219211041</v>
+      </c>
+    </row>
+    <row r="35">
+      <c r="A35" t="inlineStr">
+        <is>
+          <t>P1</t>
+        </is>
+      </c>
+      <c r="B35" t="inlineStr">
+        <is>
+          <t>P1</t>
+        </is>
+      </c>
+      <c r="C35" t="n">
+        <v>0</v>
+      </c>
+      <c r="D35" t="n">
+        <v>0</v>
+      </c>
+      <c r="E35" t="n">
+        <v>0</v>
+      </c>
+      <c r="F35" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="36">
+      <c r="A36" t="inlineStr">
+        <is>
+          <t>P1</t>
+        </is>
+      </c>
+      <c r="B36" t="inlineStr">
+        <is>
+          <t>P2</t>
+        </is>
+      </c>
+      <c r="C36" t="n">
+        <v>205.3726738091319</v>
+      </c>
+      <c r="D36" t="n">
+        <v>73.12422460304396</v>
+      </c>
+      <c r="E36" t="n">
+        <v>102.6863369045659</v>
+      </c>
+      <c r="F36" t="n">
+        <v>175.8105615076099</v>
+      </c>
+    </row>
+    <row r="37">
+      <c r="A37" t="inlineStr">
+        <is>
+          <t>P1</t>
+        </is>
+      </c>
+      <c r="B37" t="inlineStr">
+        <is>
+          <t>S1</t>
+        </is>
+      </c>
+      <c r="C37" t="n">
+        <v>1296.317108197894</v>
+      </c>
+      <c r="D37" t="n">
+        <v>436.772369399298</v>
+      </c>
+      <c r="E37" t="n">
+        <v>648.158554098947</v>
+      </c>
+      <c r="F37" t="n">
+        <v>1084.930923498245</v>
+      </c>
+    </row>
+    <row r="38">
+      <c r="A38" t="inlineStr">
+        <is>
+          <t>P1</t>
+        </is>
+      </c>
+      <c r="B38" t="inlineStr">
+        <is>
+          <t>S2</t>
+        </is>
+      </c>
+      <c r="C38" t="n">
+        <v>208.7845964459393</v>
+      </c>
+      <c r="D38" t="n">
+        <v>74.26153214864644</v>
+      </c>
+      <c r="E38" t="n">
+        <v>104.3922982229697</v>
+      </c>
+      <c r="F38" t="n">
+        <v>178.6538303716161</v>
+      </c>
+    </row>
+    <row r="39">
+      <c r="A39" t="inlineStr">
+        <is>
+          <t>P1</t>
+        </is>
+      </c>
+      <c r="B39" t="inlineStr">
+        <is>
+          <t>S3</t>
+        </is>
+      </c>
+      <c r="C39" t="n">
+        <v>192.7915133234025</v>
+      </c>
+      <c r="D39" t="n">
+        <v>68.93050444113416</v>
+      </c>
+      <c r="E39" t="n">
+        <v>96.39575666170124</v>
+      </c>
+      <c r="F39" t="n">
+        <v>165.3262611028354</v>
+      </c>
+    </row>
+    <row r="40">
+      <c r="A40" t="inlineStr">
+        <is>
+          <t>P1</t>
+        </is>
+      </c>
+      <c r="B40" t="inlineStr">
+        <is>
+          <t>S4</t>
+        </is>
+      </c>
+      <c r="C40" t="n">
+        <v>79.35219477451162</v>
+      </c>
+      <c r="D40" t="n">
+        <v>31.11739825817054</v>
+      </c>
+      <c r="E40" t="n">
+        <v>39.67609738725581</v>
+      </c>
+      <c r="F40" t="n">
+        <v>70.79349564542635</v>
+      </c>
+    </row>
+    <row r="41">
+      <c r="A41" t="inlineStr">
+        <is>
+          <t>P1</t>
+        </is>
+      </c>
+      <c r="B41" t="inlineStr">
+        <is>
+          <t>S5</t>
+        </is>
+      </c>
+      <c r="C41" t="n">
+        <v>211.7734838345068</v>
+      </c>
+      <c r="D41" t="n">
+        <v>75.2578279448356</v>
+      </c>
+      <c r="E41" t="n">
+        <v>105.8867419172534</v>
+      </c>
+      <c r="F41" t="n">
+        <v>181.144569862089</v>
+      </c>
+    </row>
+    <row r="42">
+      <c r="A42" t="inlineStr">
+        <is>
+          <t>P2</t>
+        </is>
+      </c>
+      <c r="B42" t="inlineStr">
+        <is>
+          <t>C1</t>
+        </is>
+      </c>
+      <c r="C42" t="n">
+        <v>50.61327616095006</v>
+      </c>
+      <c r="D42" t="n">
+        <v>21.53775872031669</v>
+      </c>
+      <c r="E42" t="n">
+        <v>25.30663808047503</v>
+      </c>
+      <c r="F42" t="n">
+        <v>46.84439680079171</v>
+      </c>
+    </row>
+    <row r="43">
+      <c r="A43" t="inlineStr">
+        <is>
+          <t>P2</t>
+        </is>
+      </c>
+      <c r="B43" t="inlineStr">
+        <is>
+          <t>C2</t>
+        </is>
+      </c>
+      <c r="C43" t="n">
+        <v>67.95730255244631</v>
+      </c>
+      <c r="D43" t="n">
+        <v>27.31910085081544</v>
+      </c>
+      <c r="E43" t="n">
+        <v>33.97865127622315</v>
+      </c>
+      <c r="F43" t="n">
+        <v>61.29775212703859</v>
+      </c>
+    </row>
+    <row r="44">
+      <c r="A44" t="inlineStr">
+        <is>
+          <t>P2</t>
+        </is>
+      </c>
+      <c r="B44" t="inlineStr">
+        <is>
+          <t>C3</t>
+        </is>
+      </c>
+      <c r="C44" t="n">
+        <v>154.8036398937564</v>
+      </c>
+      <c r="D44" t="n">
+        <v>56.26787996458545</v>
+      </c>
+      <c r="E44" t="n">
+        <v>77.40181994687818</v>
+      </c>
+      <c r="F44" t="n">
+        <v>133.6696999114636</v>
+      </c>
+    </row>
+    <row r="45">
+      <c r="A45" t="inlineStr">
+        <is>
+          <t>P2</t>
+        </is>
+      </c>
+      <c r="B45" t="inlineStr">
+        <is>
+          <t>P1</t>
+        </is>
+      </c>
+      <c r="C45" t="n">
+        <v>205.3726738091319</v>
+      </c>
+      <c r="D45" t="n">
+        <v>73.12422460304396</v>
+      </c>
+      <c r="E45" t="n">
+        <v>102.6863369045659</v>
+      </c>
+      <c r="F45" t="n">
+        <v>175.8105615076099</v>
+      </c>
+    </row>
+    <row r="46">
+      <c r="A46" t="inlineStr">
+        <is>
+          <t>P2</t>
+        </is>
+      </c>
+      <c r="B46" t="inlineStr">
+        <is>
+          <t>P2</t>
+        </is>
+      </c>
+      <c r="C46" t="n">
+        <v>0</v>
+      </c>
+      <c r="D46" t="n">
+        <v>0</v>
+      </c>
+      <c r="E46" t="n">
+        <v>0</v>
+      </c>
+      <c r="F46" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="47">
+      <c r="A47" t="inlineStr">
+        <is>
+          <t>P2</t>
+        </is>
+      </c>
+      <c r="B47" t="inlineStr">
+        <is>
+          <t>S1</t>
+        </is>
+      </c>
+      <c r="C47" t="n">
+        <v>1113.287259822019</v>
+      </c>
+      <c r="D47" t="n">
+        <v>375.7624199406728</v>
+      </c>
+      <c r="E47" t="n">
+        <v>556.6436299110093</v>
+      </c>
+      <c r="F47" t="n">
+        <v>932.4060498516822</v>
+      </c>
+    </row>
+    <row r="48">
+      <c r="A48" t="inlineStr">
+        <is>
+          <t>P2</t>
+        </is>
+      </c>
+      <c r="B48" t="inlineStr">
+        <is>
+          <t>S2</t>
+        </is>
+      </c>
+      <c r="C48" t="n">
+        <v>257.3213824259944</v>
+      </c>
+      <c r="D48" t="n">
+        <v>90.4404608086648</v>
+      </c>
+      <c r="E48" t="n">
+        <v>128.6606912129972</v>
+      </c>
+      <c r="F48" t="n">
+        <v>219.101152021662</v>
+      </c>
+    </row>
+    <row r="49">
+      <c r="A49" t="inlineStr">
+        <is>
+          <t>P2</t>
+        </is>
+      </c>
+      <c r="B49" t="inlineStr">
+        <is>
+          <t>S3</t>
+        </is>
+      </c>
+      <c r="C49" t="n">
+        <v>27.03932508674182</v>
+      </c>
+      <c r="D49" t="n">
+        <v>13.67977502891394</v>
+      </c>
+      <c r="E49" t="n">
+        <v>13.51966254337091</v>
+      </c>
+      <c r="F49" t="n">
+        <v>27.19943757228485</v>
+      </c>
+    </row>
+    <row r="50">
+      <c r="A50" t="inlineStr">
+        <is>
+          <t>P2</t>
+        </is>
+      </c>
+      <c r="B50" t="inlineStr">
+        <is>
+          <t>S4</t>
+        </is>
+      </c>
+      <c r="C50" t="n">
+        <v>196.9396303888934</v>
+      </c>
+      <c r="D50" t="n">
+        <v>70.31321012963113</v>
+      </c>
+      <c r="E50" t="n">
+        <v>98.4698151944467</v>
+      </c>
+      <c r="F50" t="n">
+        <v>168.7830253240778</v>
+      </c>
+    </row>
+    <row r="51">
+      <c r="A51" t="inlineStr">
+        <is>
+          <t>P2</t>
+        </is>
+      </c>
+      <c r="B51" t="inlineStr">
+        <is>
+          <t>S5</t>
+        </is>
+      </c>
+      <c r="C51" t="n">
         <v>22.58544222197883</v>
       </c>
-      <c r="D17" t="n">
+      <c r="D51" t="n">
         <v>12.19514740732628</v>
       </c>
-      <c r="E17" t="n">
+      <c r="E51" t="n">
         <v>11.29272111098942</v>
       </c>
-      <c r="F17" t="n">
+      <c r="F51" t="n">
         <v>23.48786851831569</v>
+      </c>
+    </row>
+    <row r="52">
+      <c r="A52" t="inlineStr">
+        <is>
+          <t>S1</t>
+        </is>
+      </c>
+      <c r="B52" t="inlineStr">
+        <is>
+          <t>C1</t>
+        </is>
+      </c>
+      <c r="C52" t="n">
+        <v>1159.566772494025</v>
+      </c>
+      <c r="D52" t="n">
+        <v>391.1889241646749</v>
+      </c>
+      <c r="E52" t="n">
+        <v>579.7833862470123</v>
+      </c>
+      <c r="F52" t="n">
+        <v>970.9723104116872</v>
+      </c>
+    </row>
+    <row r="53">
+      <c r="A53" t="inlineStr">
+        <is>
+          <t>S1</t>
+        </is>
+      </c>
+      <c r="B53" t="inlineStr">
+        <is>
+          <t>C2</t>
+        </is>
+      </c>
+      <c r="C53" t="n">
+        <v>1180.196966276215</v>
+      </c>
+      <c r="D53" t="n">
+        <v>398.0656554254051</v>
+      </c>
+      <c r="E53" t="n">
+        <v>590.0984831381077</v>
+      </c>
+      <c r="F53" t="n">
+        <v>988.1641385635128</v>
+      </c>
+    </row>
+    <row r="54">
+      <c r="A54" t="inlineStr">
+        <is>
+          <t>S1</t>
+        </is>
+      </c>
+      <c r="B54" t="inlineStr">
+        <is>
+          <t>C3</t>
+        </is>
+      </c>
+      <c r="C54" t="n">
+        <v>1261.990415402678</v>
+      </c>
+      <c r="D54" t="n">
+        <v>425.3301384675593</v>
+      </c>
+      <c r="E54" t="n">
+        <v>630.995207701339</v>
+      </c>
+      <c r="F54" t="n">
+        <v>1056.325346168898</v>
+      </c>
+    </row>
+    <row r="55">
+      <c r="A55" t="inlineStr">
+        <is>
+          <t>S1</t>
+        </is>
+      </c>
+      <c r="B55" t="inlineStr">
+        <is>
+          <t>P1</t>
+        </is>
+      </c>
+      <c r="C55" t="n">
+        <v>1296.317108197894</v>
+      </c>
+      <c r="D55" t="n">
+        <v>436.772369399298</v>
+      </c>
+      <c r="E55" t="n">
+        <v>648.158554098947</v>
+      </c>
+      <c r="F55" t="n">
+        <v>1084.930923498245</v>
+      </c>
+    </row>
+    <row r="56">
+      <c r="A56" t="inlineStr">
+        <is>
+          <t>S1</t>
+        </is>
+      </c>
+      <c r="B56" t="inlineStr">
+        <is>
+          <t>P2</t>
+        </is>
+      </c>
+      <c r="C56" t="n">
+        <v>1113.287259822019</v>
+      </c>
+      <c r="D56" t="n">
+        <v>375.7624199406728</v>
+      </c>
+      <c r="E56" t="n">
+        <v>556.6436299110093</v>
+      </c>
+      <c r="F56" t="n">
+        <v>932.4060498516822</v>
+      </c>
+    </row>
+    <row r="57">
+      <c r="A57" t="inlineStr">
+        <is>
+          <t>S1</t>
+        </is>
+      </c>
+      <c r="B57" t="inlineStr">
+        <is>
+          <t>S1</t>
+        </is>
+      </c>
+      <c r="C57" t="n">
+        <v>0</v>
+      </c>
+      <c r="D57" t="n">
+        <v>0</v>
+      </c>
+      <c r="E57" t="n">
+        <v>0</v>
+      </c>
+      <c r="F57" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="58">
+      <c r="A58" t="inlineStr">
+        <is>
+          <t>S1</t>
+        </is>
+      </c>
+      <c r="B58" t="inlineStr">
+        <is>
+          <t>S2</t>
+        </is>
+      </c>
+      <c r="C58" t="n">
+        <v>1353.938704942508</v>
+      </c>
+      <c r="D58" t="n">
+        <v>455.9795683141695</v>
+      </c>
+      <c r="E58" t="n">
+        <v>676.9693524712542</v>
+      </c>
+      <c r="F58" t="n">
+        <v>1132.948920785424</v>
+      </c>
+    </row>
+    <row r="59">
+      <c r="A59" t="inlineStr">
+        <is>
+          <t>S1</t>
+        </is>
+      </c>
+      <c r="B59" t="inlineStr">
+        <is>
+          <t>S3</t>
+        </is>
+      </c>
+      <c r="C59" t="n">
+        <v>1114.492386682703</v>
+      </c>
+      <c r="D59" t="n">
+        <v>376.1641288942343</v>
+      </c>
+      <c r="E59" t="n">
+        <v>557.2461933413515</v>
+      </c>
+      <c r="F59" t="n">
+        <v>933.4103222355858</v>
+      </c>
+    </row>
+    <row r="60">
+      <c r="A60" t="inlineStr">
+        <is>
+          <t>S1</t>
+        </is>
+      </c>
+      <c r="B60" t="inlineStr">
+        <is>
+          <t>S4</t>
+        </is>
+      </c>
+      <c r="C60" t="n">
+        <v>1244.433611924373</v>
+      </c>
+      <c r="D60" t="n">
+        <v>419.4778706414576</v>
+      </c>
+      <c r="E60" t="n">
+        <v>622.2168059621865</v>
+      </c>
+      <c r="F60" t="n">
+        <v>1041.694676603644</v>
+      </c>
+    </row>
+    <row r="61">
+      <c r="A61" t="inlineStr">
+        <is>
+          <t>S1</t>
+        </is>
+      </c>
+      <c r="B61" t="inlineStr">
+        <is>
+          <t>S5</t>
+        </is>
+      </c>
+      <c r="C61" t="n">
+        <v>1098.089095994044</v>
+      </c>
+      <c r="D61" t="n">
+        <v>370.696365331348</v>
+      </c>
+      <c r="E61" t="n">
+        <v>549.0445479970221</v>
+      </c>
+      <c r="F61" t="n">
+        <v>919.74091332837</v>
+      </c>
+    </row>
+    <row r="62">
+      <c r="A62" t="inlineStr">
+        <is>
+          <t>S2</t>
+        </is>
+      </c>
+      <c r="B62" t="inlineStr">
+        <is>
+          <t>C1</t>
+        </is>
+      </c>
+      <c r="C62" t="n">
+        <v>206.7285173493552</v>
+      </c>
+      <c r="D62" t="n">
+        <v>73.57617244978508</v>
+      </c>
+      <c r="E62" t="n">
+        <v>103.3642586746776</v>
+      </c>
+      <c r="F62" t="n">
+        <v>176.9404311244627</v>
+      </c>
+    </row>
+    <row r="63">
+      <c r="A63" t="inlineStr">
+        <is>
+          <t>S2</t>
+        </is>
+      </c>
+      <c r="B63" t="inlineStr">
+        <is>
+          <t>C2</t>
+        </is>
+      </c>
+      <c r="C63" t="n">
+        <v>203.9719900298204</v>
+      </c>
+      <c r="D63" t="n">
+        <v>72.65733000994013</v>
+      </c>
+      <c r="E63" t="n">
+        <v>101.9859950149102</v>
+      </c>
+      <c r="F63" t="n">
+        <v>174.6433250248503</v>
+      </c>
+    </row>
+    <row r="64">
+      <c r="A64" t="inlineStr">
+        <is>
+          <t>S2</t>
+        </is>
+      </c>
+      <c r="B64" t="inlineStr">
+        <is>
+          <t>C3</t>
+        </is>
+      </c>
+      <c r="C64" t="n">
+        <v>171.0808992653463</v>
+      </c>
+      <c r="D64" t="n">
+        <v>61.69363308844878</v>
+      </c>
+      <c r="E64" t="n">
+        <v>85.54044963267316</v>
+      </c>
+      <c r="F64" t="n">
+        <v>147.2340827211219</v>
+      </c>
+    </row>
+    <row r="65">
+      <c r="A65" t="inlineStr">
+        <is>
+          <t>S2</t>
+        </is>
+      </c>
+      <c r="B65" t="inlineStr">
+        <is>
+          <t>P1</t>
+        </is>
+      </c>
+      <c r="C65" t="n">
+        <v>208.7845964459393</v>
+      </c>
+      <c r="D65" t="n">
+        <v>74.26153214864644</v>
+      </c>
+      <c r="E65" t="n">
+        <v>104.3922982229697</v>
+      </c>
+      <c r="F65" t="n">
+        <v>178.6538303716161</v>
+      </c>
+    </row>
+    <row r="66">
+      <c r="A66" t="inlineStr">
+        <is>
+          <t>S2</t>
+        </is>
+      </c>
+      <c r="B66" t="inlineStr">
+        <is>
+          <t>P2</t>
+        </is>
+      </c>
+      <c r="C66" t="n">
+        <v>257.3213824259944</v>
+      </c>
+      <c r="D66" t="n">
+        <v>90.4404608086648</v>
+      </c>
+      <c r="E66" t="n">
+        <v>128.6606912129972</v>
+      </c>
+      <c r="F66" t="n">
+        <v>219.101152021662</v>
+      </c>
+    </row>
+    <row r="67">
+      <c r="A67" t="inlineStr">
+        <is>
+          <t>S2</t>
+        </is>
+      </c>
+      <c r="B67" t="inlineStr">
+        <is>
+          <t>S1</t>
+        </is>
+      </c>
+      <c r="C67" t="n">
+        <v>1353.938704942508</v>
+      </c>
+      <c r="D67" t="n">
+        <v>455.9795683141695</v>
+      </c>
+      <c r="E67" t="n">
+        <v>676.9693524712542</v>
+      </c>
+      <c r="F67" t="n">
+        <v>1132.948920785424</v>
+      </c>
+    </row>
+    <row r="68">
+      <c r="A68" t="inlineStr">
+        <is>
+          <t>S2</t>
+        </is>
+      </c>
+      <c r="B68" t="inlineStr">
+        <is>
+          <t>S2</t>
+        </is>
+      </c>
+      <c r="C68" t="n">
+        <v>0</v>
+      </c>
+      <c r="D68" t="n">
+        <v>0</v>
+      </c>
+      <c r="E68" t="n">
+        <v>0</v>
+      </c>
+      <c r="F68" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="69">
+      <c r="A69" t="inlineStr">
+        <is>
+          <t>S2</t>
+        </is>
+      </c>
+      <c r="B69" t="inlineStr">
+        <is>
+          <t>S3</t>
+        </is>
+      </c>
+      <c r="C69" t="n">
+        <v>268.232696248839</v>
+      </c>
+      <c r="D69" t="n">
+        <v>94.07756541627967</v>
+      </c>
+      <c r="E69" t="n">
+        <v>134.1163481244195</v>
+      </c>
+      <c r="F69" t="n">
+        <v>228.1939135406992</v>
+      </c>
+    </row>
+    <row r="70">
+      <c r="A70" t="inlineStr">
+        <is>
+          <t>S2</t>
+        </is>
+      </c>
+      <c r="B70" t="inlineStr">
+        <is>
+          <t>S4</t>
+        </is>
+      </c>
+      <c r="C70" t="n">
+        <v>280.086682487771</v>
+      </c>
+      <c r="D70" t="n">
+        <v>98.02889416259035</v>
+      </c>
+      <c r="E70" t="n">
+        <v>140.0433412438855</v>
+      </c>
+      <c r="F70" t="n">
+        <v>238.0722354064759</v>
+      </c>
+    </row>
+    <row r="71">
+      <c r="A71" t="inlineStr">
+        <is>
+          <t>S2</t>
+        </is>
+      </c>
+      <c r="B71" t="inlineStr">
+        <is>
+          <t>S5</t>
+        </is>
+      </c>
+      <c r="C71" t="n">
+        <v>278.0551892359258</v>
+      </c>
+      <c r="D71" t="n">
+        <v>97.3517297453086</v>
+      </c>
+      <c r="E71" t="n">
+        <v>139.0275946179629</v>
+      </c>
+      <c r="F71" t="n">
+        <v>236.3793243632715</v>
+      </c>
+    </row>
+    <row r="72">
+      <c r="A72" t="inlineStr">
+        <is>
+          <t>S3</t>
+        </is>
+      </c>
+      <c r="B72" t="inlineStr">
+        <is>
+          <t>C1</t>
+        </is>
+      </c>
+      <c r="C72" t="n">
+        <v>65.89157990019301</v>
+      </c>
+      <c r="D72" t="n">
+        <v>26.63052663339767</v>
+      </c>
+      <c r="E72" t="n">
+        <v>32.9457899500965</v>
+      </c>
+      <c r="F72" t="n">
+        <v>59.57631658349418</v>
+      </c>
+    </row>
+    <row r="73">
+      <c r="A73" t="inlineStr">
+        <is>
+          <t>S3</t>
+        </is>
+      </c>
+      <c r="B73" t="inlineStr">
+        <is>
+          <t>C2</t>
+        </is>
+      </c>
+      <c r="C73" t="n">
+        <v>67.60376858924941</v>
+      </c>
+      <c r="D73" t="n">
+        <v>27.20125619641647</v>
+      </c>
+      <c r="E73" t="n">
+        <v>33.80188429462471</v>
+      </c>
+      <c r="F73" t="n">
+        <v>61.00314049104118</v>
+      </c>
+    </row>
+    <row r="74">
+      <c r="A74" t="inlineStr">
+        <is>
+          <t>S3</t>
+        </is>
+      </c>
+      <c r="B74" t="inlineStr">
+        <is>
+          <t>C3</t>
+        </is>
+      </c>
+      <c r="C74" t="n">
+        <v>148.1909253635272</v>
+      </c>
+      <c r="D74" t="n">
+        <v>54.06364178784239</v>
+      </c>
+      <c r="E74" t="n">
+        <v>74.09546268176359</v>
+      </c>
+      <c r="F74" t="n">
+        <v>128.159104469606</v>
+      </c>
+    </row>
+    <row r="75">
+      <c r="A75" t="inlineStr">
+        <is>
+          <t>S3</t>
+        </is>
+      </c>
+      <c r="B75" t="inlineStr">
+        <is>
+          <t>P1</t>
+        </is>
+      </c>
+      <c r="C75" t="n">
+        <v>192.7915133234025</v>
+      </c>
+      <c r="D75" t="n">
+        <v>68.93050444113416</v>
+      </c>
+      <c r="E75" t="n">
+        <v>96.39575666170124</v>
+      </c>
+      <c r="F75" t="n">
+        <v>165.3262611028354</v>
+      </c>
+    </row>
+    <row r="76">
+      <c r="A76" t="inlineStr">
+        <is>
+          <t>S3</t>
+        </is>
+      </c>
+      <c r="B76" t="inlineStr">
+        <is>
+          <t>P2</t>
+        </is>
+      </c>
+      <c r="C76" t="n">
+        <v>27.03932508674182</v>
+      </c>
+      <c r="D76" t="n">
+        <v>13.67977502891394</v>
+      </c>
+      <c r="E76" t="n">
+        <v>13.51966254337091</v>
+      </c>
+      <c r="F76" t="n">
+        <v>27.19943757228485</v>
+      </c>
+    </row>
+    <row r="77">
+      <c r="A77" t="inlineStr">
+        <is>
+          <t>S3</t>
+        </is>
+      </c>
+      <c r="B77" t="inlineStr">
+        <is>
+          <t>S1</t>
+        </is>
+      </c>
+      <c r="C77" t="n">
+        <v>1114.492386682703</v>
+      </c>
+      <c r="D77" t="n">
+        <v>376.1641288942343</v>
+      </c>
+      <c r="E77" t="n">
+        <v>557.2461933413515</v>
+      </c>
+      <c r="F77" t="n">
+        <v>933.4103222355858</v>
+      </c>
+    </row>
+    <row r="78">
+      <c r="A78" t="inlineStr">
+        <is>
+          <t>S3</t>
+        </is>
+      </c>
+      <c r="B78" t="inlineStr">
+        <is>
+          <t>S2</t>
+        </is>
+      </c>
+      <c r="C78" t="n">
+        <v>268.232696248839</v>
+      </c>
+      <c r="D78" t="n">
+        <v>94.07756541627967</v>
+      </c>
+      <c r="E78" t="n">
+        <v>134.1163481244195</v>
+      </c>
+      <c r="F78" t="n">
+        <v>228.1939135406992</v>
+      </c>
+    </row>
+    <row r="79">
+      <c r="A79" t="inlineStr">
+        <is>
+          <t>S3</t>
+        </is>
+      </c>
+      <c r="B79" t="inlineStr">
+        <is>
+          <t>S3</t>
+        </is>
+      </c>
+      <c r="C79" t="n">
+        <v>0</v>
+      </c>
+      <c r="D79" t="n">
+        <v>0</v>
+      </c>
+      <c r="E79" t="n">
+        <v>0</v>
+      </c>
+      <c r="F79" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="80">
+      <c r="A80" t="inlineStr">
+        <is>
+          <t>S3</t>
+        </is>
+      </c>
+      <c r="B80" t="inlineStr">
+        <is>
+          <t>S4</t>
+        </is>
+      </c>
+      <c r="C80" t="n">
+        <v>175.8617587171285</v>
+      </c>
+      <c r="D80" t="n">
+        <v>63.28725290570951</v>
+      </c>
+      <c r="E80" t="n">
+        <v>87.93087935856427</v>
+      </c>
+      <c r="F80" t="n">
+        <v>151.2181322642738</v>
+      </c>
+    </row>
+    <row r="81">
+      <c r="A81" t="inlineStr">
+        <is>
+          <t>S3</t>
+        </is>
+      </c>
+      <c r="B81" t="inlineStr">
+        <is>
+          <t>S5</t>
+        </is>
+      </c>
+      <c r="C81" t="n">
+        <v>19.27072199596897</v>
+      </c>
+      <c r="D81" t="n">
+        <v>11.09024066532299</v>
+      </c>
+      <c r="E81" t="n">
+        <v>9.635360997984485</v>
+      </c>
+      <c r="F81" t="n">
+        <v>20.72560166330748</v>
+      </c>
+    </row>
+    <row r="82">
+      <c r="A82" t="inlineStr">
+        <is>
+          <t>S4</t>
+        </is>
+      </c>
+      <c r="B82" t="inlineStr">
+        <is>
+          <t>C1</t>
+        </is>
+      </c>
+      <c r="C82" t="n">
+        <v>191.3610883898892</v>
+      </c>
+      <c r="D82" t="n">
+        <v>68.45369612996306</v>
+      </c>
+      <c r="E82" t="n">
+        <v>95.68054419494459</v>
+      </c>
+      <c r="F82" t="n">
+        <v>164.1342403249076</v>
+      </c>
+    </row>
+    <row r="83">
+      <c r="A83" t="inlineStr">
+        <is>
+          <t>S4</t>
+        </is>
+      </c>
+      <c r="B83" t="inlineStr">
+        <is>
+          <t>C2</t>
+        </is>
+      </c>
+      <c r="C83" t="n">
+        <v>152.8377121278224</v>
+      </c>
+      <c r="D83" t="n">
+        <v>55.61257070927415</v>
+      </c>
+      <c r="E83" t="n">
+        <v>76.41885606391122</v>
+      </c>
+      <c r="F83" t="n">
+        <v>132.0314267731854</v>
+      </c>
+    </row>
+    <row r="84">
+      <c r="A84" t="inlineStr">
+        <is>
+          <t>S4</t>
+        </is>
+      </c>
+      <c r="B84" t="inlineStr">
+        <is>
+          <t>C3</t>
+        </is>
+      </c>
+      <c r="C84" t="n">
+        <v>112.2871622400843</v>
+      </c>
+      <c r="D84" t="n">
+        <v>42.09572074669477</v>
+      </c>
+      <c r="E84" t="n">
+        <v>56.14358112004216</v>
+      </c>
+      <c r="F84" t="n">
+        <v>98.23930186673694</v>
+      </c>
+    </row>
+    <row r="85">
+      <c r="A85" t="inlineStr">
+        <is>
+          <t>S4</t>
+        </is>
+      </c>
+      <c r="B85" t="inlineStr">
+        <is>
+          <t>P1</t>
+        </is>
+      </c>
+      <c r="C85" t="n">
+        <v>79.35219477451162</v>
+      </c>
+      <c r="D85" t="n">
+        <v>31.11739825817054</v>
+      </c>
+      <c r="E85" t="n">
+        <v>39.67609738725581</v>
+      </c>
+      <c r="F85" t="n">
+        <v>70.79349564542635</v>
+      </c>
+    </row>
+    <row r="86">
+      <c r="A86" t="inlineStr">
+        <is>
+          <t>S4</t>
+        </is>
+      </c>
+      <c r="B86" t="inlineStr">
+        <is>
+          <t>P2</t>
+        </is>
+      </c>
+      <c r="C86" t="n">
+        <v>196.9396303888934</v>
+      </c>
+      <c r="D86" t="n">
+        <v>70.31321012963113</v>
+      </c>
+      <c r="E86" t="n">
+        <v>98.4698151944467</v>
+      </c>
+      <c r="F86" t="n">
+        <v>168.7830253240778</v>
+      </c>
+    </row>
+    <row r="87">
+      <c r="A87" t="inlineStr">
+        <is>
+          <t>S4</t>
+        </is>
+      </c>
+      <c r="B87" t="inlineStr">
+        <is>
+          <t>S1</t>
+        </is>
+      </c>
+      <c r="C87" t="n">
+        <v>1244.433611924373</v>
+      </c>
+      <c r="D87" t="n">
+        <v>419.4778706414576</v>
+      </c>
+      <c r="E87" t="n">
+        <v>622.2168059621865</v>
+      </c>
+      <c r="F87" t="n">
+        <v>1041.694676603644</v>
+      </c>
+    </row>
+    <row r="88">
+      <c r="A88" t="inlineStr">
+        <is>
+          <t>S4</t>
+        </is>
+      </c>
+      <c r="B88" t="inlineStr">
+        <is>
+          <t>S2</t>
+        </is>
+      </c>
+      <c r="C88" t="n">
+        <v>280.086682487771</v>
+      </c>
+      <c r="D88" t="n">
+        <v>98.02889416259035</v>
+      </c>
+      <c r="E88" t="n">
+        <v>140.0433412438855</v>
+      </c>
+      <c r="F88" t="n">
+        <v>238.0722354064759</v>
+      </c>
+    </row>
+    <row r="89">
+      <c r="A89" t="inlineStr">
+        <is>
+          <t>S4</t>
+        </is>
+      </c>
+      <c r="B89" t="inlineStr">
+        <is>
+          <t>S3</t>
+        </is>
+      </c>
+      <c r="C89" t="n">
+        <v>175.8617587171285</v>
+      </c>
+      <c r="D89" t="n">
+        <v>63.28725290570951</v>
+      </c>
+      <c r="E89" t="n">
+        <v>87.93087935856427</v>
+      </c>
+      <c r="F89" t="n">
+        <v>151.2181322642738</v>
+      </c>
+    </row>
+    <row r="90">
+      <c r="A90" t="inlineStr">
+        <is>
+          <t>S4</t>
+        </is>
+      </c>
+      <c r="B90" t="inlineStr">
+        <is>
+          <t>S4</t>
+        </is>
+      </c>
+      <c r="C90" t="n">
+        <v>0</v>
+      </c>
+      <c r="D90" t="n">
+        <v>0</v>
+      </c>
+      <c r="E90" t="n">
+        <v>0</v>
+      </c>
+      <c r="F90" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="91">
+      <c r="A91" t="inlineStr">
+        <is>
+          <t>S4</t>
+        </is>
+      </c>
+      <c r="B91" t="inlineStr">
+        <is>
+          <t>S5</t>
+        </is>
+      </c>
+      <c r="C91" t="n">
+        <v>194.6235671453617</v>
+      </c>
+      <c r="D91" t="n">
+        <v>69.54118904845389</v>
+      </c>
+      <c r="E91" t="n">
+        <v>97.31178357268084</v>
+      </c>
+      <c r="F91" t="n">
+        <v>166.8529726211347</v>
+      </c>
+    </row>
+    <row r="92">
+      <c r="A92" t="inlineStr">
+        <is>
+          <t>S5</t>
+        </is>
+      </c>
+      <c r="B92" t="inlineStr">
+        <is>
+          <t>C1</t>
+        </is>
+      </c>
+      <c r="C92" t="n">
+        <v>71.95941646118726</v>
+      </c>
+      <c r="D92" t="n">
+        <v>28.65313882039575</v>
+      </c>
+      <c r="E92" t="n">
+        <v>35.97970823059363</v>
+      </c>
+      <c r="F92" t="n">
+        <v>64.63284705098938</v>
+      </c>
+    </row>
+    <row r="93">
+      <c r="A93" t="inlineStr">
+        <is>
+          <t>S5</t>
+        </is>
+      </c>
+      <c r="B93" t="inlineStr">
+        <is>
+          <t>C2</t>
+        </is>
+      </c>
+      <c r="C93" t="n">
+        <v>82.28463421703982</v>
+      </c>
+      <c r="D93" t="n">
+        <v>32.0948780723466</v>
+      </c>
+      <c r="E93" t="n">
+        <v>41.14231710851991</v>
+      </c>
+      <c r="F93" t="n">
+        <v>73.23719518086651</v>
+      </c>
+    </row>
+    <row r="94">
+      <c r="A94" t="inlineStr">
+        <is>
+          <t>S5</t>
+        </is>
+      </c>
+      <c r="B94" t="inlineStr">
+        <is>
+          <t>C3</t>
+        </is>
+      </c>
+      <c r="C94" t="n">
+        <v>165.7915884437255</v>
+      </c>
+      <c r="D94" t="n">
+        <v>59.93052948124182</v>
+      </c>
+      <c r="E94" t="n">
+        <v>82.89579422186274</v>
+      </c>
+      <c r="F94" t="n">
+        <v>142.8263237031045</v>
+      </c>
+    </row>
+    <row r="95">
+      <c r="A95" t="inlineStr">
+        <is>
+          <t>S5</t>
+        </is>
+      </c>
+      <c r="B95" t="inlineStr">
+        <is>
+          <t>P1</t>
+        </is>
+      </c>
+      <c r="C95" t="n">
+        <v>211.7734838345068</v>
+      </c>
+      <c r="D95" t="n">
+        <v>75.2578279448356</v>
+      </c>
+      <c r="E95" t="n">
+        <v>105.8867419172534</v>
+      </c>
+      <c r="F95" t="n">
+        <v>181.144569862089</v>
+      </c>
+    </row>
+    <row r="96">
+      <c r="A96" t="inlineStr">
+        <is>
+          <t>S5</t>
+        </is>
+      </c>
+      <c r="B96" t="inlineStr">
+        <is>
+          <t>P2</t>
+        </is>
+      </c>
+      <c r="C96" t="n">
+        <v>22.58544222197883</v>
+      </c>
+      <c r="D96" t="n">
+        <v>12.19514740732628</v>
+      </c>
+      <c r="E96" t="n">
+        <v>11.29272111098942</v>
+      </c>
+      <c r="F96" t="n">
+        <v>23.48786851831569</v>
+      </c>
+    </row>
+    <row r="97">
+      <c r="A97" t="inlineStr">
+        <is>
+          <t>S5</t>
+        </is>
+      </c>
+      <c r="B97" t="inlineStr">
+        <is>
+          <t>S1</t>
+        </is>
+      </c>
+      <c r="C97" t="n">
+        <v>1098.089095994044</v>
+      </c>
+      <c r="D97" t="n">
+        <v>370.696365331348</v>
+      </c>
+      <c r="E97" t="n">
+        <v>549.0445479970221</v>
+      </c>
+      <c r="F97" t="n">
+        <v>919.74091332837</v>
+      </c>
+    </row>
+    <row r="98">
+      <c r="A98" t="inlineStr">
+        <is>
+          <t>S5</t>
+        </is>
+      </c>
+      <c r="B98" t="inlineStr">
+        <is>
+          <t>S2</t>
+        </is>
+      </c>
+      <c r="C98" t="n">
+        <v>278.0551892359258</v>
+      </c>
+      <c r="D98" t="n">
+        <v>97.3517297453086</v>
+      </c>
+      <c r="E98" t="n">
+        <v>139.0275946179629</v>
+      </c>
+      <c r="F98" t="n">
+        <v>236.3793243632715</v>
+      </c>
+    </row>
+    <row r="99">
+      <c r="A99" t="inlineStr">
+        <is>
+          <t>S5</t>
+        </is>
+      </c>
+      <c r="B99" t="inlineStr">
+        <is>
+          <t>S3</t>
+        </is>
+      </c>
+      <c r="C99" t="n">
+        <v>19.27072199596897</v>
+      </c>
+      <c r="D99" t="n">
+        <v>11.09024066532299</v>
+      </c>
+      <c r="E99" t="n">
+        <v>9.635360997984485</v>
+      </c>
+      <c r="F99" t="n">
+        <v>20.72560166330748</v>
+      </c>
+    </row>
+    <row r="100">
+      <c r="A100" t="inlineStr">
+        <is>
+          <t>S5</t>
+        </is>
+      </c>
+      <c r="B100" t="inlineStr">
+        <is>
+          <t>S4</t>
+        </is>
+      </c>
+      <c r="C100" t="n">
+        <v>194.6235671453617</v>
+      </c>
+      <c r="D100" t="n">
+        <v>69.54118904845389</v>
+      </c>
+      <c r="E100" t="n">
+        <v>97.31178357268084</v>
+      </c>
+      <c r="F100" t="n">
+        <v>166.8529726211347</v>
+      </c>
+    </row>
+    <row r="101">
+      <c r="A101" t="inlineStr">
+        <is>
+          <t>S5</t>
+        </is>
+      </c>
+      <c r="B101" t="inlineStr">
+        <is>
+          <t>S5</t>
+        </is>
+      </c>
+      <c r="C101" t="n">
+        <v>0</v>
+      </c>
+      <c r="D101" t="n">
+        <v>0</v>
+      </c>
+      <c r="E101" t="n">
+        <v>0</v>
+      </c>
+      <c r="F101" t="n">
+        <v>0</v>
       </c>
     </row>
   </sheetData>

</xml_diff>